<commit_message>
Created new decals and footprints with 3D models
</commit_message>
<xml_diff>
--- a/Hardware/BOM/Arduino_LCD_Experimenter_Shield_BOM.xlsx
+++ b/Hardware/BOM/Arduino_LCD_Experimenter_Shield_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>BOM
 Item</t>
@@ -59,9 +59,6 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>MCP7940M-I/ST</t>
-  </si>
-  <si>
     <t>CAT24M01-SO8</t>
   </si>
   <si>
@@ -108,6 +105,60 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>BK-912</t>
+  </si>
+  <si>
+    <t>Memory Protection Devices</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>C1608C0G1H080D080AA</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>APT1608YC</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>LED (0603)</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>OSRAM</t>
+  </si>
+  <si>
+    <t>LED (0805)</t>
+  </si>
+  <si>
+    <t>LY R976-PS-36</t>
+  </si>
+  <si>
+    <t>BAV70LT1G</t>
+  </si>
+  <si>
+    <t>Fairchild</t>
+  </si>
+  <si>
+    <t>BAT54C</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>MCP23008-E/SS</t>
   </si>
 </sst>
 </file>
@@ -139,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,11 +213,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -197,6 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +567,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,10 +615,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="3"/>
@@ -572,7 +635,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="3"/>
@@ -585,13 +648,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="3"/>
@@ -608,7 +671,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="3"/>
@@ -621,11 +684,11 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="3"/>
@@ -635,14 +698,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -655,13 +718,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -674,11 +737,11 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="11"/>
@@ -688,14 +751,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="11"/>
@@ -704,10 +767,16 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="11"/>
     </row>
@@ -715,10 +784,16 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F12" s="13"/>
       <c r="G12" s="11"/>
     </row>
@@ -726,10 +801,18 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13" s="3"/>
     </row>
@@ -737,10 +820,18 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="F14" s="12"/>
       <c r="G14" s="3"/>
     </row>
@@ -748,19 +839,32 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>

</xml_diff>